<commit_message>
Testing unit tests relying on spectra
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1b_CO2_Fluid_Inclusions/Weak_Diads.xlsx
+++ b/docs/Examples/Example1b_CO2_Fluid_Inclusions/Weak_Diads.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:AU17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,46 @@
           <t>Diad1_Gauss_Sigma</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Asym50</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Asym70</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Yuan2017_sym_factor</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Remigi2021_BSF</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Asym50</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Asym70</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Yuan2017_sym_factor</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Remigi2021_BSF</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -736,6 +776,30 @@
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="n">
+        <v>1.164133738602162</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>1.152173913043523</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.1922834017836951</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.0008571089448770777</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1.100917431193286</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1.100000000000032</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.1027222787810408</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.0004185099443979589</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -843,6 +907,30 @@
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="n">
+        <v>1.181008902076529</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>1.146551724137428</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.2139112653169737</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.0009137605674561974</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1.081081081080656</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>1.081775700934434</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.08279008964124143</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.0004555797481215617</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -950,6 +1038,30 @@
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="n">
+        <v>1.198198198198423</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>1.185185185185261</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.2350882955196955</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.0006390089314212232</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1.06547619047562</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>1.067129629629676</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.06721912718399045</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.0003130828167376919</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1045,6 +1157,30 @@
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="n">
+        <v>1.195035460993019</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1.20111731843574</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.1829373502616893</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.02019587356651059</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1.034482758620562</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1.03888888888852</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.02574252342936353</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.009673999294495873</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1152,6 +1288,30 @@
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="n">
+        <v>1.252631578946804</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>1.266846361185536</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.2436567203689979</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.001527742367305308</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>1.095057034220433</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>1.122507122507193</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.08687053902164894</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.0008885840855582906</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1259,6 +1419,30 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="n">
+        <v>1.201954397394592</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>1.201511335012676</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.2020226264871046</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.002408408218673916</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>1.06716417910465</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>1.088642659279925</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.06234023522498912</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.001366294128249545</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1360,6 +1544,30 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="n">
+        <v>1.003597122302353</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>1.002645502645645</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0.003388154343009955</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.004003132965718732</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>1.251937984496013</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>1.28398791540778</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.2162185216442824</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.002122158418979997</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1461,6 +1669,30 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="n">
+        <v>1.017595307917657</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>1.027310924369817</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.02052391063450729</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.003601925827545564</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>1.221476510067057</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>1.22137404580167</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.227293600785559</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.001836225772890855</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1568,6 +1800,30 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="n">
+        <v>1.094674556212968</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>1.095541401273929</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>0.1123638294330259</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.0006100426740246082</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>1.197411003235526</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>1.190123456789631</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.2029290416787086</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.0003006820035996373</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1675,6 +1931,30 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="n">
+        <v>1.025568181818422</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>1.053388090348928</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.03077567239018532</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.0007172586770451544</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>1.203225806451472</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>1.193627450980329</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.2120469227446246</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.0003537435869755437</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1782,6 +2062,30 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="n">
+        <v>1.026086956521594</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1.008196721311367</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.03089089429699293</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.001907789716365235</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>1.223333333333295</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>1.218592964823898</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.2310084308933085</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.0009513085296379747</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1889,6 +2193,30 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="n">
+        <v>1.022922636102848</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1.010183299389007</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.02746718630240945</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.002555081465427714</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>1.217821782178126</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1.212499999999719</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0.2244890929404168</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.001258444643877306</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1996,6 +2324,30 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr"/>
       <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="n">
+        <v>1.025714285714142</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>1.033482142857151</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.02792417226723898</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.003273157864424728</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>1.038732394366109</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>1.035989717223308</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0.03785469975302655</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.001747704912994523</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2103,6 +2455,30 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="n">
+        <v>1.101744186046138</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1.068131868131711</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.1156179298024332</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>0.001701159774999307</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>1.03092783505186</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>1.047619047619528</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0.03091937550983918</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>0.000919340054609549</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2210,6 +2586,30 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="n">
+        <v>1.016574585635515</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1.008528784648363</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.01856866585007859</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.002757223678063495</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>1.03496503496491</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>1.043701799485593</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0.03405848687296949</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.00152434322579094</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2317,6 +2717,30 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="n">
+        <v>1.007462686567234</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1.070610687022875</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.01000199511166949</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.002807459033431672</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>1.195286195286329</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>1.20749999999967</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0.2050119700710883</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.001203286975286477</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>